<commit_message>
Issue #317, procedure examples
</commit_message>
<xml_diff>
--- a/Codegen/src/Documentation/CodegenStudy.xlsx
+++ b/Codegen/src/Documentation/CodegenStudy.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="132">
   <si>
     <t>Blank line</t>
   </si>
@@ -1137,6 +1137,274 @@
   </si>
   <si>
     <t>If Node is generated, generate the code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000000  declare procedure Check private
+000000           input  Date1  type Date
+000000           output Result pic X.
+000000   procedure division.
+000000     if Date1 = spaces
+000000         move 'Y' to result
+000000     else
+000000         move 'N' to result
+000000     end-if.
+000000  end-declare  
+000000  move a to b
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000  declare procedure Check private
+000000           input  Date1  type Date
+000000           output Result pic X.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+000000   move a to b
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">* declare procedure Check private
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">*          input  Date1  type Date
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>*          output Result pic X.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000 IDENTIFICATION DIVISION.
+000000 PROGRAM-ID. ca65c9a2.
+000000 DATA DIVISION.
+000000 LINKAGE SECTION.
+000000 01 Date1.
+000000     02 Year  pic X(04).
+000000     02 Month pic X(02).
+000000     02 Day   pic X(02).
+000000 01 Result pic X.
+000000 procedure division using Date1
+000000                          Result.
+000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">     if Date1 = spaces
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">         move 'Y' to result
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">     else
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">         move 'N' to result
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">     end-if.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+000000 END PROGRAM ca65c9a2.</t>
+    </r>
+  </si>
+  <si>
+    <t>000000      call Procedure input  MyDate1
+000000                     output MyResult</t>
+  </si>
+  <si>
+    <r>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>*     call Procedure input  MyDate1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>*                    output MyResult</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+000000      call 'ca65c9a2' using MyDate1
+000000                            MyResult
+000000      end-call</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1689,13 +1957,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,20 +2553,14 @@
       <c r="J32" s="27"/>
     </row>
     <row r="33" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="9" t="s">
+      <c r="A33" s="6"/>
+      <c r="G33" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="H33" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I33" s="8"/>
-      <c r="J33" s="28"/>
+      <c r="J33" s="27"/>
     </row>
     <row r="34" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -2336,183 +2598,195 @@
       </c>
       <c r="J35" s="27"/>
     </row>
-    <row r="36" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="9" t="s">
+    <row r="36" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="G36" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="H36" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I36" s="8"/>
-      <c r="J36" s="28"/>
-    </row>
-    <row r="37" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
+      <c r="J36" s="27"/>
+    </row>
+    <row r="37" spans="1:10" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="G37" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J37" s="27"/>
+    </row>
+    <row r="38" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I38" s="8"/>
+      <c r="J38" s="28"/>
+    </row>
+    <row r="39" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B39" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C39" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="14"/>
-      <c r="E37" s="15" t="s">
+      <c r="D39" s="8"/>
+      <c r="E39" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F39" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G37" s="16" t="s">
+      <c r="G39" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="H39" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="I37" s="14"/>
-      <c r="J37" s="29"/>
-    </row>
-    <row r="38" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I38" s="4"/>
-      <c r="J38" s="26"/>
-    </row>
-    <row r="39" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>98</v>
       </c>
       <c r="I39" s="8"/>
       <c r="J39" s="28"/>
     </row>
-    <row r="40" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13" t="s">
+    <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I40" s="4"/>
+      <c r="J40" s="26"/>
+    </row>
+    <row r="41" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I41" s="8"/>
+      <c r="J41" s="28"/>
+    </row>
+    <row r="42" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B42" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C42" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="14"/>
-      <c r="E40" s="15" t="s">
+      <c r="D42" s="14"/>
+      <c r="E42" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F42" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G40" s="16" t="s">
+      <c r="G42" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="H40" s="16" t="s">
+      <c r="H42" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="I40" s="14" t="s">
+      <c r="I42" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="J40" s="29" t="s">
+      <c r="J42" s="29" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E43" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F43" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G42" s="1" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G44" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G43" s="1" t="s">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G45" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="E44" s="10" t="s">
+    <row r="46" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="E46" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F46" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G45" s="1"/>
-      <c r="H45" s="25"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G46" s="1"/>
-      <c r="H46" s="25"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G47" s="1"/>
@@ -2549,6 +2823,14 @@
     <row r="55" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G55" s="1"/>
       <c r="H55" s="25"/>
+    </row>
+    <row r="56" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G56" s="1"/>
+      <c r="H56" s="25"/>
+    </row>
+    <row r="57" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G57" s="1"/>
+      <c r="H57" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Issue #317, fix some align bug and added a new case for COPY and procedure declaration
</commit_message>
<xml_diff>
--- a/Codegen/src/Documentation/CodegenStudy.xlsx
+++ b/Codegen/src/Documentation/CodegenStudy.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="134">
   <si>
     <t>Blank line</t>
   </si>
@@ -386,16 +386,6 @@
 000000                       to b   move c to d</t>
   </si>
   <si>
-    <t>000000     move a 
-000000                       to b   move c to 
-000000                                                                 d</t>
-  </si>
-  <si>
-    <t>000000     move z to y    move a 
-000000                       to b   move c to 
-000000                                                                 d</t>
-  </si>
-  <si>
     <t>Cobol 85  code on single line</t>
   </si>
   <si>
@@ -444,165 +434,10 @@
     <t>000000      set MyBool to true</t>
   </si>
   <si>
-    <r>
-      <t>000000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>*             Set MyBool To true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>000000               Set MyBool-true To true</t>
-    </r>
-  </si>
-  <si>
     <t>000000      set MyBool to true  set MyBool2 to true</t>
   </si>
   <si>
-    <r>
-      <t>000000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>*             Set MyBool To true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">000000               Set MyBool-true To true
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>000000*             Set MyBool2 To true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-000000               Set MyBool2-true To true</t>
-    </r>
-  </si>
-  <si>
     <t>Generated code (for Alpha)</t>
-  </si>
-  <si>
-    <r>
-      <t>000000 COPY MyCopy. 
-000000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>*                                     Set MyBool To true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>000000                                       Set MyBool-true To true</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>000000 COPY MyCopy. 
-000000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>*                                    Set MyBool 
-000000*                           To true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>000000      Set MyBool-true To true</t>
-    </r>
   </si>
   <si>
     <t>TypeCobol code on multiple lines</t>
@@ -956,42 +791,6 @@
   </si>
   <si>
     <t>Set MyBool-true To true is too long, so push it on the left until it fit</t>
-  </si>
-  <si>
-    <r>
-      <t>000000 COPY 
-000000      MyCopy. 
-000000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>*                          Set MyBool 
-000000*                        To true</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>000000               Set MyBool-true To true</t>
-    </r>
   </si>
   <si>
     <t>Align Set MyBool-true To true to the original position of Set</t>
@@ -1153,6 +952,511 @@
 </t>
   </si>
   <si>
+    <t>000000      call Procedure input  MyDate1
+000000                     output MyResult</t>
+  </si>
+  <si>
+    <r>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>*     call Procedure input  MyDate1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>*                    output MyResult</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+000000      call 'ca65c9a2' using MyDate1
+000000                            MyResult
+000000      end-call</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>000000 COPY MyCopy. 
+000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>*             Set MyBool To true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000              Set MyBool-true To true</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>000000 COPY MyCopy. 
+000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>*             Set MyBool 
+000000*                        To true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000              Set MyBool-true To true</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>000000 COPY 
+000000      MyCopy. 
+000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>*             Set MyBool 
+000000*                        To true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000              Set MyBool-true To true</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>*     Set MyBool To true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000      Set MyBool-true To true</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>*     Set MyBool To true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">000000      Set MyBool-true To true
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000*     Set MyBool2 To true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+000000      Set MyBool2-true To true</t>
+    </r>
+  </si>
+  <si>
+    <t>000000     move a 
+000000                       to b   move c to 
+000000                                        d</t>
+  </si>
+  <si>
+    <t>000000     move z to y    move a 
+000000                       to b   move c to 
+000000                                        d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000000  declare procedure Check2 private
+000000           input  Date1  type Date.
+000000   data division.
+000000   working-storage section.
+000000   01 DATS20. COPY YDATS20.
+000000   procedure division.
+000000     if Date1 = spaces
+000000         move 'Y' to result
+000000     else
+000000         move 'N' to result
+000000     end-if.
+000000  end-declare  
+000000  move a to b
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000  declare procedure Check2 private
+000000           input  Date1  type Date.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+000000   move a to b
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">* declare procedure Check2 private
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>*          input  Date1  type Date.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">000000 IDENTIFICATION DIVISION.
+000000 PROGRAM-ID. wz6789b2.
+000000 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>data division.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+000000 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>working-storage section.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+000000 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>01 DATS20. COPY YDATS20.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+000000 LINKAGE SECTION.
+000000 01 Date1.
+000000     02 Year  pic X(04).
+000000     02 Month pic X(02).
+000000     02 Day   pic X(02).
+000000 procedure division using Date1.
+000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">     if Date1 = spaces
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">         move 'Y' to result
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">     else
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">         move 'N' to result
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">     end-if.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
+000000 END PROGRAM wz6789b2.</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1248,7 +1552,7 @@
         <rFont val="Courier New"/>
         <family val="3"/>
       </rPr>
-      <t>000000 IDENTIFICATION DIVISION.
+      <t xml:space="preserve">000000 IDENTIFICATION DIVISION.
 000000 PROGRAM-ID. ca65c9a2.
 000000 DATA DIVISION.
 000000 LINKAGE SECTION.
@@ -1256,7 +1560,25 @@
 000000     02 Year  pic X(04).
 000000     02 Month pic X(02).
 000000     02 Day   pic X(02).
-000000 01 Result pic X.
+000000 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>01 Result pic X.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">
 000000 procedure division using Date1
 000000                          Result.
 000000</t>
@@ -1355,55 +1677,6 @@
       </rPr>
       <t xml:space="preserve">
 000000 END PROGRAM ca65c9a2.</t>
-    </r>
-  </si>
-  <si>
-    <t>000000      call Procedure input  MyDate1
-000000                     output MyResult</t>
-  </si>
-  <si>
-    <r>
-      <t>000000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>*     call Procedure input  MyDate1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-000000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>*                    output MyResult</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-000000      call 'ca65c9a2' using MyDate1
-000000                            MyResult
-000000      end-call</t>
     </r>
   </si>
 </sst>
@@ -1957,13 +2230,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G35" sqref="G35"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1974,7 +2247,7 @@
     <col min="4" max="4" width="42.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" style="10" customWidth="1"/>
     <col min="6" max="6" width="18.140625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="66.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="66.85546875" style="23" customWidth="1"/>
     <col min="8" max="8" width="68.140625" style="23" customWidth="1"/>
     <col min="9" max="9" width="68.28515625" style="2" customWidth="1"/>
     <col min="10" max="10" width="36.85546875" style="2" customWidth="1"/>
@@ -2018,13 +2291,13 @@
         <v>11</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2250,7 +2523,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="26"/>
     </row>
-    <row r="14" spans="1:10" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -2261,7 +2534,7 @@
         <v>45</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="28"/>
@@ -2364,13 +2637,13 @@
       </c>
       <c r="J20" s="27"/>
     </row>
-    <row r="21" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="G21" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="J21" s="27"/>
     </row>
@@ -2385,16 +2658,16 @@
         <v>52</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="28" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>2</v>
@@ -2490,17 +2763,17 @@
       </c>
       <c r="J28" s="27"/>
     </row>
-    <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="G29" s="1" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="J29" s="27"/>
     </row>
-    <row r="30" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -2508,17 +2781,17 @@
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="9" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="I30" s="8"/>
       <c r="J30" s="28"/>
     </row>
     <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>2</v>
@@ -2534,10 +2807,10 @@
         <v>28</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="26"/>
@@ -2545,26 +2818,26 @@
     <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="G32" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
       <c r="J32" s="27"/>
     </row>
     <row r="33" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="G33" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="J33" s="27"/>
     </row>
     <row r="34" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>2</v>
@@ -2580,10 +2853,10 @@
         <v>28</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="26"/>
@@ -2591,206 +2864,212 @@
     <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="G35" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J35" s="27"/>
     </row>
     <row r="36" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="G36" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="J36" s="27"/>
     </row>
     <row r="37" spans="1:10" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="G37" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="J37" s="27"/>
     </row>
-    <row r="38" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="H38" s="9" t="s">
+    <row r="38" spans="1:10" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="G38" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I38" s="8"/>
-      <c r="J38" s="28"/>
-    </row>
-    <row r="39" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>91</v>
-      </c>
+      <c r="H38" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J38" s="27"/>
+    </row>
+    <row r="39" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
       <c r="D39" s="8"/>
-      <c r="E39" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>28</v>
-      </c>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
       <c r="G39" s="9" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="I39" s="8"/>
       <c r="J39" s="28"/>
     </row>
-    <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="8"/>
+      <c r="E40" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I40" s="8"/>
+      <c r="J40" s="28"/>
+    </row>
+    <row r="41" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I41" s="4"/>
+      <c r="J41" s="26"/>
+    </row>
+    <row r="42" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="I42" s="8"/>
+      <c r="J42" s="28"/>
+    </row>
+    <row r="43" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="11" t="s">
+      <c r="D43" s="14"/>
+      <c r="E43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F43" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="G43" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="H43" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="I40" s="4"/>
-      <c r="J40" s="26"/>
-    </row>
-    <row r="41" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="H41" s="9" t="s">
+      <c r="I43" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="I41" s="8"/>
-      <c r="J41" s="28"/>
-    </row>
-    <row r="42" spans="1:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="14" t="s">
+      <c r="J43" s="29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D42" s="14"/>
-      <c r="E42" s="15" t="s">
+      <c r="B44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F42" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G42" s="16" t="s">
+      <c r="F44" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H42" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="J42" s="29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G44" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="H44" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G45" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="E46" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G46" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="E47" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F47" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G47" s="1"/>
-      <c r="H47" s="25"/>
+      <c r="G47" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G48" s="1"/>
@@ -2831,6 +3110,10 @@
     <row r="57" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G57" s="1"/>
       <c r="H57" s="25"/>
+    </row>
+    <row r="58" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G58" s="1"/>
+      <c r="H58" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2945,65 +3228,65 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>